<commit_message>
Added COVID-19 incubation analysis to 2_Data_Cleaning_and_Preprocessing.ipynb
</commit_message>
<xml_diff>
--- a/Data_Wrangling_Python/examples/ex1.xlsx
+++ b/Data_Wrangling_Python/examples/ex1.xlsx
@@ -8,28 +8,27 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>message</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Message</t>
   </si>
   <si>
     <t>hello</t>
@@ -482,94 +481,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>